<commit_message>
commit edited sd and testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dataforhackathon.xlsx
+++ b/src/test/resources/Testdata/dataforhackathon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitf\eclipse-workspace\LMSHackathon_Phase2\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9367EAB-735F-4EFE-A603-83FDAE87689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C6763F-EC80-4299-8640-CC6155DA6A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="5565" windowWidth="20460" windowHeight="10890" xr2:uid="{A29177D1-063F-476E-95C9-478361BFC846}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A29177D1-063F-476E-95C9-478361BFC846}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>testid</t>
   </si>
@@ -175,6 +175,21 @@
   </si>
   <si>
     <t>(validstudentid)</t>
+  </si>
+  <si>
+    <t>Dditems</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>late</t>
+  </si>
+  <si>
+    <t>excused</t>
   </si>
 </sst>
 </file>
@@ -551,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A23F17A-2DCD-486D-A8CE-5FEF602873A9}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,6 +1005,23 @@
         <v>42</v>
       </c>
     </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>